<commit_message>
Updated Tasks and Userstories
</commit_message>
<xml_diff>
--- a/Doku/Tasks.xlsx
+++ b/Doku/Tasks.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Masood/Dropbox/Studienprojekt Master/Projektmanagement/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16140"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,9 +13,6 @@
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -193,9 +185,6 @@
     <t>Auswahl des Modells, nicht eingeben der ID per Hand</t>
   </si>
   <si>
-    <t>Daniel, Christina</t>
-  </si>
-  <si>
     <t>Model als BPMN speichern</t>
   </si>
   <si>
@@ -371,6 +360,9 @@
   </si>
   <si>
     <t>Ergebnisse zippen und bereitstellen</t>
+  </si>
+  <si>
+    <t>Christina, Jenny, Masood</t>
   </si>
 </sst>
 </file>
@@ -618,7 +610,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="45">
     <dxf>
@@ -1459,17 +1451,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="187" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="28.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="4:8" x14ac:dyDescent="0.2">
@@ -1595,10 +1587,10 @@
         <v>39</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D15" s="3"/>
       <c r="E15" s="16" t="s">
         <v>19</v>
@@ -1611,7 +1603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D16" s="3"/>
       <c r="E16" s="16" t="s">
         <v>20</v>
@@ -1623,7 +1615,7 @@
         <v>14</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.2">
@@ -1679,7 +1671,7 @@
     <row r="21" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D21" s="3"/>
       <c r="E21" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="5" t="s">
@@ -1698,7 +1690,7 @@
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
       <c r="E23" s="16" t="s">
         <v>41</v>
@@ -1711,7 +1703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D24" s="3"/>
       <c r="E24" s="16" t="s">
         <v>42</v>
@@ -1721,10 +1713,10 @@
         <v>43</v>
       </c>
       <c r="H24" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" s="3"/>
       <c r="E25" s="16" t="s">
         <v>44</v>
@@ -1737,7 +1729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D26" s="3"/>
       <c r="E26" s="16" t="s">
         <v>45</v>
@@ -1747,10 +1739,10 @@
         <v>43</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D27" s="3"/>
       <c r="E27" s="16" t="s">
         <v>46</v>
@@ -1763,7 +1755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D28" s="3"/>
       <c r="E28" s="16" t="s">
         <v>47</v>
@@ -1773,10 +1765,10 @@
         <v>43</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D29" s="3"/>
       <c r="E29" s="4" t="s">
         <v>52</v>
@@ -1785,13 +1777,13 @@
         <v>53</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D30" s="3"/>
       <c r="E30" s="16" t="s">
         <v>48</v>
@@ -1804,7 +1796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
       <c r="E31" s="16" t="s">
         <v>49</v>
@@ -1814,10 +1806,10 @@
         <v>43</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D32" s="3"/>
       <c r="E32" s="16" t="s">
         <v>50</v>
@@ -1827,10 +1819,10 @@
         <v>24</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D33" s="3"/>
       <c r="E33" s="16" t="s">
         <v>51</v>
@@ -1840,13 +1832,13 @@
         <v>43</v>
       </c>
       <c r="H33" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D34" s="3"/>
       <c r="E34" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="17" t="s">
@@ -1856,10 +1848,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D35" s="3"/>
       <c r="E35" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="17" t="s">
@@ -1869,36 +1861,36 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D36" s="3"/>
       <c r="E36" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H36" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D37" s="3"/>
       <c r="E37" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H37" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D38" s="3"/>
       <c r="E38" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="17" t="s">
@@ -1908,13 +1900,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D39" s="3"/>
       <c r="E39" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G39" s="17" t="s">
         <v>24</v>
@@ -1923,172 +1915,172 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D40" s="3"/>
       <c r="E40" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="17" t="s">
         <v>16</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D41" s="3"/>
       <c r="E41" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="17" t="s">
         <v>16</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D42" s="3"/>
       <c r="E42" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="17" t="s">
         <v>16</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D43" s="3"/>
       <c r="E43" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H43" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D44" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
     </row>
-    <row r="45" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D45" s="7"/>
       <c r="E45" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D47" s="3"/>
       <c r="E47" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D48" s="3"/>
       <c r="E48" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="5" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D49" s="3"/>
       <c r="E49" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D50" s="3"/>
       <c r="E50" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="51" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D51" s="3"/>
       <c r="E51" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D52" s="3"/>
       <c r="E52" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D53" s="14" t="s">
         <v>36</v>
       </c>
@@ -2097,13 +2089,13 @@
       <c r="G53" s="14"/>
       <c r="H53" s="14"/>
     </row>
-    <row r="54" spans="4:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D54" s="3"/>
       <c r="E54" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G54" s="17" t="s">
         <v>24</v>
@@ -2112,10 +2104,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D55" s="3"/>
       <c r="E55" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="17" t="s">
@@ -2125,10 +2117,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D56" s="3"/>
       <c r="E56" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4" t="s">
@@ -2138,10 +2130,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D57" s="3"/>
       <c r="E57" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4" t="s">
@@ -2151,13 +2143,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D58" s="3"/>
       <c r="E58" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>24</v>
@@ -2166,10 +2158,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="4:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D59" s="7"/>
       <c r="E59" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="4" t="s">
@@ -2179,20 +2171,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D60" s="3"/>
       <c r="E60" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="61" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D61" s="14" t="s">
         <v>27</v>
       </c>
@@ -2201,13 +2193,13 @@
       <c r="G61" s="14"/>
       <c r="H61" s="14"/>
     </row>
-    <row r="62" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D62" s="3"/>
       <c r="E62" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F62" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>24</v>
@@ -2216,7 +2208,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D63" s="3"/>
       <c r="E63" s="4" t="s">
         <v>28</v>
@@ -2229,10 +2221,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D64" s="3"/>
       <c r="E64" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="17" t="s">
@@ -2242,7 +2234,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D65" s="3"/>
       <c r="E65" s="4" t="s">
         <v>29</v>
@@ -2255,16 +2247,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D66" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E66" s="21"/>
       <c r="F66" s="21"/>
       <c r="G66" s="22"/>
       <c r="H66" s="23"/>
     </row>
-    <row r="67" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D67" s="3"/>
       <c r="E67" s="4" t="s">
         <v>23</v>
@@ -2277,7 +2269,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D68" s="3"/>
       <c r="E68" s="4" t="s">
         <v>25</v>
@@ -2286,16 +2278,16 @@
         <v>26</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D69" s="3"/>
       <c r="E69" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="5" t="s">
@@ -2305,10 +2297,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D70" s="3"/>
       <c r="E70" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="24" t="s">
@@ -2318,10 +2310,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D71" s="3"/>
       <c r="E71" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F71" s="4"/>
       <c r="G71" s="5" t="s">
@@ -2331,10 +2323,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D72" s="3"/>
       <c r="E72" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F72" s="4"/>
       <c r="G72" s="24" t="s">
@@ -2344,10 +2336,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D73" s="3"/>
       <c r="E73" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F73" s="4"/>
       <c r="G73" s="5" t="s">
@@ -2357,10 +2349,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D74" s="3"/>
       <c r="E74" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F74" s="4"/>
       <c r="G74" s="24" t="s">
@@ -2370,10 +2362,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D75" s="3"/>
       <c r="E75" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="5" t="s">
@@ -2383,10 +2375,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D76" s="3"/>
       <c r="E76" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="24" t="s">
@@ -2396,10 +2388,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D77" s="3"/>
       <c r="E77" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="5" t="s">
@@ -2409,10 +2401,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="78" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D78" s="3"/>
       <c r="E78" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="24" t="s">
@@ -2422,10 +2414,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="79" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D79" s="3"/>
       <c r="E79" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="5" t="s">
@@ -2435,10 +2427,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="80" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D80" s="3"/>
       <c r="E80" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="24" t="s">
@@ -2448,10 +2440,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="81" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D81" s="3"/>
       <c r="E81" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="24" t="s">
@@ -2461,10 +2453,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D82" s="7"/>
       <c r="E82" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F82" s="8"/>
       <c r="G82" s="26" t="s">
@@ -2474,80 +2466,80 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D83" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E83" s="14"/>
       <c r="F83" s="14"/>
       <c r="G83" s="14"/>
       <c r="H83" s="14"/>
     </row>
-    <row r="84" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D84" s="7"/>
       <c r="E84" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F84" s="8"/>
       <c r="G84" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H84" s="25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="85" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D85" s="7"/>
       <c r="E85" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F85" s="8"/>
       <c r="G85" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H85" s="25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="86" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="4:8" ht="45" x14ac:dyDescent="0.25">
       <c r="D86" s="7"/>
       <c r="E86" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F86" s="8"/>
       <c r="G86" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H86" s="25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="87" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D87" s="3"/>
       <c r="E87" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F87" s="4"/>
       <c r="G87" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="88" spans="4:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D88" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E88" s="21"/>
       <c r="F88" s="21"/>
       <c r="G88" s="22"/>
       <c r="H88" s="23"/>
     </row>
-    <row r="89" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D89" s="3"/>
       <c r="E89" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F89" s="4"/>
       <c r="G89" s="5" t="s">
@@ -2557,14 +2549,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="4:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D90" s="7"/>
       <c r="E90" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F90" s="8"/>
       <c r="G90" s="9" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="H90" s="25" t="s">
         <v>18</v>
@@ -2719,7 +2711,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2731,7 +2723,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Tasklist from Dropbox
</commit_message>
<xml_diff>
--- a/Doku/Tasks.xlsx
+++ b/Doku/Tasks.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="142">
   <si>
     <t>Task</t>
   </si>
@@ -441,6 +441,12 @@
   </si>
   <si>
     <t>Verschoben da AngularBinding gestört wird durch Sandbox</t>
+  </si>
+  <si>
+    <t>Bei Konflikten mit Version als popup</t>
+  </si>
+  <si>
+    <t>Save Modal einfügen</t>
   </si>
 </sst>
 </file>
@@ -636,7 +642,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -690,13 +696,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="60">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1323,14 +1392,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B5:F113" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="52" tableBorderDxfId="51" totalsRowBorderDxfId="50">
-  <autoFilter ref="B5:F113"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B5:F114" totalsRowShown="0" headerRowDxfId="59" headerRowBorderDxfId="58" tableBorderDxfId="57" totalsRowBorderDxfId="56">
+  <autoFilter ref="B5:F114"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Task" dataDxfId="49"/>
-    <tableColumn id="2" name="Subtask" dataDxfId="48"/>
-    <tableColumn id="3" name="Kommentar" dataDxfId="47"/>
-    <tableColumn id="4" name="Bearbeiter" dataDxfId="46"/>
-    <tableColumn id="5" name="Status" dataDxfId="45"/>
+    <tableColumn id="1" name="Task" dataDxfId="55"/>
+    <tableColumn id="2" name="Subtask" dataDxfId="54"/>
+    <tableColumn id="3" name="Kommentar" dataDxfId="53"/>
+    <tableColumn id="4" name="Bearbeiter" dataDxfId="52"/>
+    <tableColumn id="5" name="Status" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1623,10 +1692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:F113"/>
+  <dimension ref="B5:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,7 +1833,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="16" t="s">
         <v>14</v>
@@ -1877,7 +1946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="16" t="s">
         <v>33</v>
@@ -1903,7 +1972,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="16" t="s">
         <v>35</v>
@@ -1916,7 +1985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="16" t="s">
         <v>36</v>
@@ -1929,7 +1998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="16" t="s">
         <v>37</v>
@@ -1983,7 +2052,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="C32" s="16" t="s">
         <v>39</v>
@@ -1996,7 +2065,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
       <c r="C33" s="4" t="s">
         <v>102</v>
@@ -2011,21 +2080,23 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
-      <c r="C34" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="17" t="s">
-        <v>124</v>
+      <c r="C34" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>128</v>
       </c>
       <c r="F34" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="17" t="s">
@@ -2035,10 +2106,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="C36" s="16" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="17" t="s">
@@ -2048,27 +2119,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="C37" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="16"/>
+      <c r="E38" s="17" t="s">
         <v>126</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="3"/>
-      <c r="C38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="17" t="s">
-        <v>124</v>
       </c>
       <c r="F38" s="19" t="s">
         <v>6</v>
@@ -2077,7 +2148,7 @@
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="C39" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="17" t="s">
@@ -2090,7 +2161,7 @@
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="17" t="s">
@@ -2103,7 +2174,7 @@
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="17" t="s">
@@ -2116,7 +2187,7 @@
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
       <c r="C42" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="17" t="s">
@@ -2126,14 +2197,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
       <c r="C43" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D43" s="4"/>
       <c r="E43" s="17" t="s">
         <v>124</v>
       </c>
@@ -2141,13 +2210,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
       <c r="C44" s="4" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>114</v>
+        <v>49</v>
       </c>
       <c r="E44" s="17" t="s">
         <v>124</v>
@@ -2159,10 +2228,10 @@
     <row r="45" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
       <c r="C45" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="E45" s="17" t="s">
         <v>124</v>
@@ -2174,11 +2243,13 @@
     <row r="46" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
       <c r="C46" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D46" s="4"/>
+        <v>115</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="E46" s="17" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F46" s="19" t="s">
         <v>6</v>
@@ -2187,7 +2258,7 @@
     <row r="47" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
       <c r="C47" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="17" t="s">
@@ -2200,7 +2271,7 @@
     <row r="48" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="17" t="s">
@@ -2213,11 +2284,11 @@
     <row r="49" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="3"/>
       <c r="C49" s="4" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F49" s="19" t="s">
         <v>6</v>
@@ -2226,10 +2297,10 @@
     <row r="50" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
       <c r="C50" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D50" s="4"/>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="17" t="s">
         <v>129</v>
       </c>
       <c r="F50" s="19" t="s">
@@ -2239,42 +2310,42 @@
     <row r="51" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="3"/>
       <c r="C51" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+      <c r="C52" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="17" t="s">
+      <c r="D52" s="4"/>
+      <c r="E52" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="F51" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="14" t="s">
+      <c r="F52" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-    </row>
-    <row r="53" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="7"/>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+    </row>
+    <row r="54" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="7"/>
+      <c r="C54" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="D53" s="8"/>
-      <c r="E53" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B54" s="7"/>
-      <c r="C54" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="5" t="s">
@@ -2284,12 +2355,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B55" s="3"/>
-      <c r="C55" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D55" s="4"/>
+    <row r="55" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B55" s="7"/>
+      <c r="C55" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D55" s="8"/>
       <c r="E55" s="5" t="s">
         <v>128</v>
       </c>
@@ -2299,8 +2370,8 @@
     </row>
     <row r="56" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
-      <c r="C56" s="8" t="s">
-        <v>77</v>
+      <c r="C56" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="5" t="s">
@@ -2312,21 +2383,21 @@
     </row>
     <row r="57" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B58" s="3"/>
+      <c r="C58" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
-      <c r="C58" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="5" t="s">
@@ -2336,12 +2407,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
-      <c r="C59" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D59" s="4"/>
+      <c r="C59" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D59" s="8"/>
       <c r="E59" s="5" t="s">
         <v>133</v>
       </c>
@@ -2351,8 +2422,8 @@
     </row>
     <row r="60" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
-      <c r="C60" s="8" t="s">
-        <v>81</v>
+      <c r="C60" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="5" t="s">
@@ -2364,60 +2435,60 @@
     </row>
     <row r="61" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" s="3"/>
-      <c r="C61" s="4" t="s">
-        <v>111</v>
+      <c r="C61" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="5" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
       <c r="C62" s="4" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+      <c r="C63" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D63" s="4"/>
+      <c r="E63" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F62" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="14" t="s">
+      <c r="F63" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-    </row>
-    <row r="64" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B64" s="3"/>
-      <c r="C64" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E64" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+    </row>
+    <row r="65" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B65" s="3"/>
       <c r="C65" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D65" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="E65" s="17" t="s">
         <v>124</v>
       </c>
@@ -2428,20 +2499,20 @@
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="3"/>
       <c r="C66" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D66" s="4"/>
-      <c r="E66" s="4" t="s">
+      <c r="E66" s="17" t="s">
         <v>124</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="3"/>
       <c r="C67" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4" t="s">
@@ -2454,48 +2525,48 @@
     <row r="68" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
       <c r="C68" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+      <c r="C69" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D69" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E68" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B69" s="7"/>
-      <c r="C69" s="4" t="s">
+      <c r="E69" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B70" s="7"/>
+      <c r="C70" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-      <c r="C70" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B71" s="3"/>
       <c r="C71" s="4" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4" t="s">
@@ -2505,36 +2576,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B72" s="14" t="s">
+    <row r="72" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B72" s="3"/>
+      <c r="C72" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-    </row>
-    <row r="73" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-      <c r="C73" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
     </row>
     <row r="74" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B74" s="3"/>
       <c r="C74" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D74" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="E74" s="5" t="s">
         <v>124</v>
       </c>
@@ -2545,11 +2616,11 @@
     <row r="75" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B75" s="3"/>
       <c r="C75" s="4" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="D75" s="4"/>
-      <c r="E75" s="17" t="s">
-        <v>134</v>
+      <c r="E75" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>6</v>
@@ -2558,61 +2629,61 @@
     <row r="76" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D76" s="4"/>
+      <c r="E76" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+      <c r="C77" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D76" s="4"/>
-      <c r="E76" s="5" t="s">
+      <c r="D77" s="4"/>
+      <c r="E77" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F76" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="14" t="s">
+      <c r="F77" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
-      <c r="E77" s="22"/>
-      <c r="F77" s="23"/>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-      <c r="C78" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D78" s="4"/>
-      <c r="E78" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="23"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="3"/>
       <c r="C79" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D79" s="20" t="s">
-        <v>20</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D79" s="4"/>
       <c r="E79" s="5" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="3"/>
       <c r="C80" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D80" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="D80" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="E80" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>6</v>
@@ -2621,10 +2692,10 @@
     <row r="81" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="3"/>
       <c r="C81" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D81" s="4"/>
-      <c r="E81" s="24" t="s">
+      <c r="E81" s="5" t="s">
         <v>135</v>
       </c>
       <c r="F81" s="6" t="s">
@@ -2634,88 +2705,88 @@
     <row r="82" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B82" s="3"/>
       <c r="C82" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D82" s="4"/>
-      <c r="E82" s="5" t="s">
+      <c r="E82" s="24" t="s">
         <v>135</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B83" s="3"/>
       <c r="C83" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D83" s="4"/>
-      <c r="E83" s="24" t="s">
+      <c r="E83" s="5" t="s">
         <v>135</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B84" s="3"/>
       <c r="C84" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D84" s="4"/>
-      <c r="E84" s="5" t="s">
-        <v>136</v>
+      <c r="E84" s="24" t="s">
+        <v>135</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B85" s="3"/>
       <c r="C85" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D85" s="4"/>
-      <c r="E85" s="24" t="s">
-        <v>135</v>
+      <c r="E85" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B86" s="3"/>
       <c r="C86" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D86" s="4"/>
-      <c r="E86" s="5" t="s">
+      <c r="E86" s="24" t="s">
         <v>135</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B87" s="3"/>
       <c r="C87" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D87" s="4"/>
-      <c r="E87" s="24" t="s">
+      <c r="E87" s="5" t="s">
         <v>135</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B88" s="3"/>
       <c r="C88" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D88" s="4"/>
-      <c r="E88" s="5" t="s">
+      <c r="E88" s="24" t="s">
         <v>135</v>
       </c>
       <c r="F88" s="6" t="s">
@@ -2725,10 +2796,10 @@
     <row r="89" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B89" s="3"/>
       <c r="C89" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D89" s="4"/>
-      <c r="E89" s="24" t="s">
+      <c r="E89" s="5" t="s">
         <v>135</v>
       </c>
       <c r="F89" s="6" t="s">
@@ -2738,81 +2809,81 @@
     <row r="90" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="3"/>
       <c r="C90" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D90" s="4"/>
-      <c r="E90" s="5" t="s">
+      <c r="E90" s="24" t="s">
         <v>135</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B91" s="3"/>
       <c r="C91" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D91" s="4"/>
-      <c r="E91" s="24" t="s">
+      <c r="E91" s="5" t="s">
         <v>135</v>
       </c>
       <c r="F91" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B92" s="3"/>
       <c r="C92" s="4" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B93" s="3"/>
+      <c r="C93" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D93" s="4"/>
+      <c r="E93" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="F92" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B93" s="7"/>
-      <c r="C93" s="8" t="s">
+      <c r="F93" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B94" s="7"/>
+      <c r="C94" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D93" s="8"/>
-      <c r="E93" s="26" t="s">
+      <c r="D94" s="8"/>
+      <c r="E94" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="F93" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B94" s="14" t="s">
+      <c r="F94" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C94" s="14"/>
-      <c r="D94" s="14"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="14"/>
-    </row>
-    <row r="95" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B95" s="7"/>
-      <c r="C95" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D95" s="8"/>
-      <c r="E95" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F95" s="25" t="s">
-        <v>6</v>
-      </c>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
     </row>
     <row r="96" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B96" s="7"/>
       <c r="C96" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D96" s="8"/>
       <c r="E96" s="9" t="s">
@@ -2822,10 +2893,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B97" s="7"/>
       <c r="C97" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D97" s="8"/>
       <c r="E97" s="9" t="s">
@@ -2835,23 +2906,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B98" s="3"/>
-      <c r="C98" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D98" s="4"/>
-      <c r="E98" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F98" s="6" t="s">
+    <row r="98" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B98" s="7"/>
+      <c r="C98" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D98" s="8"/>
+      <c r="E98" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F98" s="25" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="99" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="3"/>
       <c r="C99" s="4" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="5" t="s">
@@ -2861,32 +2932,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B100" s="14" t="s">
+    <row r="100" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B100" s="3"/>
+      <c r="C100" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D100" s="4"/>
+      <c r="E100" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B101" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C100" s="21"/>
-      <c r="D100" s="21"/>
-      <c r="E100" s="22"/>
-      <c r="F100" s="23"/>
-    </row>
-    <row r="101" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B101" s="3"/>
-      <c r="C101" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D101" s="4"/>
-      <c r="E101" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F101" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C101" s="21"/>
+      <c r="D101" s="21"/>
+      <c r="E101" s="22"/>
+      <c r="F101" s="23"/>
+    </row>
+    <row r="102" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B102" s="3"/>
       <c r="C102" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="5" t="s">
@@ -2899,7 +2970,7 @@
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="3"/>
       <c r="C103" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="5" t="s">
@@ -2912,7 +2983,7 @@
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" s="3"/>
       <c r="C104" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="5" t="s">
@@ -2922,45 +2993,45 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105" s="3"/>
       <c r="C105" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B106" s="3"/>
+      <c r="C106" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D106" s="4"/>
+      <c r="E106" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F105" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B106" s="14" t="s">
+      <c r="F106" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B107" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C106" s="21"/>
-      <c r="D106" s="21"/>
-      <c r="E106" s="22"/>
-      <c r="F106" s="23"/>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B107" s="3"/>
-      <c r="C107" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D107" s="4"/>
-      <c r="E107" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F107" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="108" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C107" s="21"/>
+      <c r="D107" s="21"/>
+      <c r="E107" s="22"/>
+      <c r="F107" s="23"/>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108" s="3"/>
       <c r="C108" s="4" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="5" t="s">
@@ -2973,7 +3044,7 @@
     <row r="109" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B109" s="3"/>
       <c r="C109" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="5" t="s">
@@ -2986,7 +3057,7 @@
     <row r="110" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B110" s="3"/>
       <c r="C110" s="4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="5" t="s">
@@ -2997,212 +3068,236 @@
       </c>
     </row>
     <row r="111" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B111" s="7"/>
-      <c r="C111" s="8" t="s">
+      <c r="B111" s="3"/>
+      <c r="C111" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D111" s="4"/>
+      <c r="E111" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B112" s="7"/>
+      <c r="C112" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D111" s="8"/>
-      <c r="E111" s="9" t="s">
+      <c r="D112" s="8"/>
+      <c r="E112" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F111" s="25" t="s">
+      <c r="F112" s="25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B112" s="3"/>
-      <c r="C112" s="4" t="s">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B113" s="3"/>
+      <c r="C113" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D112" s="4"/>
-      <c r="E112" s="5" t="s">
+      <c r="D113" s="4"/>
+      <c r="E113" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F112" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B113" s="27"/>
-      <c r="C113" s="8" t="s">
+      <c r="F113" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B114" s="27"/>
+      <c r="C114" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D113" s="8"/>
-      <c r="E113" s="28" t="s">
+      <c r="D114" s="8"/>
+      <c r="E114" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="F113" s="6" t="s">
+      <c r="F114" s="6" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F114:F1048576 F107:F110 F33 F36:F49 F51:F81 F1:F24 F95:F99">
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+  <conditionalFormatting sqref="F115:F1048576 F108:F111 F33 F37:F50 F52:F82 F1:F24 F96:F100">
+    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:F26">
-    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27:F30">
-    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31:F32">
-    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F82:F83">
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+  <conditionalFormatting sqref="F83:F84">
+    <cfRule type="cellIs" dxfId="38" priority="34" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F84:F85">
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+  <conditionalFormatting sqref="F85:F86">
+    <cfRule type="cellIs" dxfId="35" priority="31" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F86:F87">
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+  <conditionalFormatting sqref="F87:F88">
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F88:F89">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+  <conditionalFormatting sqref="F89:F90">
+    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F90:F93">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+  <conditionalFormatting sqref="F91:F94">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F111:F112">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+  <conditionalFormatting sqref="F112:F113">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F57:F61">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+  <conditionalFormatting sqref="F58:F62">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F113">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+  <conditionalFormatting sqref="F114">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34:F35">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+  <conditionalFormatting sqref="F35:F36">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F50">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+  <conditionalFormatting sqref="F51">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F101:F105">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="F102:F106">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"Offen"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F34">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"Wartend"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Erledigt"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D79" r:id="rId1"/>
+    <hyperlink ref="D80" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Fixes for Administration page
</commit_message>
<xml_diff>
--- a/Doku/Tasks.xlsx
+++ b/Doku/Tasks.xlsx
@@ -425,21 +425,6 @@
     <t>Granit Gecaj, Masood Ahmed</t>
   </si>
   <si>
-    <t>Jenny Espich, Christina Frank, Daniel Lackmann, Granit Gecaj, Masood Ahmed, Markus Schmidtner</t>
-  </si>
-  <si>
-    <t>Jenny Espich</t>
-  </si>
-  <si>
-    <t>Jenny Espich, Markus Schmidtner</t>
-  </si>
-  <si>
-    <t>Christina Frank, Jenny Espich, Masood Ahmed</t>
-  </si>
-  <si>
-    <t>Daniel Lackmann, Jenny Espich</t>
-  </si>
-  <si>
     <t>Verschoben da AngularBinding gestört wird durch Sandbox</t>
   </si>
   <si>
@@ -447,6 +432,21 @@
   </si>
   <si>
     <t>Save Modal einfügen</t>
+  </si>
+  <si>
+    <t>Jennifer Espich, Christina Frank, Daniel Lackmann, Granit Gecaj, Masood Ahmed, Markus Schmidtner</t>
+  </si>
+  <si>
+    <t>Jennifer Espich</t>
+  </si>
+  <si>
+    <t>Jennifer Espich, Markus Schmidtner</t>
+  </si>
+  <si>
+    <t>Christina Frank, Jennifer Espich, Masood Ahmed</t>
+  </si>
+  <si>
+    <t>Daniel Lackmann, Jennifer Espich</t>
   </si>
 </sst>
 </file>
@@ -705,517 +705,7 @@
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="57">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1377,6 +867,486 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1392,14 +1362,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B5:F114" totalsRowShown="0" headerRowDxfId="59" headerRowBorderDxfId="58" tableBorderDxfId="57" totalsRowBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B5:F114" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="B5:F114"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Task" dataDxfId="55"/>
-    <tableColumn id="2" name="Subtask" dataDxfId="54"/>
-    <tableColumn id="3" name="Kommentar" dataDxfId="53"/>
-    <tableColumn id="4" name="Bearbeiter" dataDxfId="52"/>
-    <tableColumn id="5" name="Status" dataDxfId="51"/>
+    <tableColumn id="1" name="Task" dataDxfId="4"/>
+    <tableColumn id="2" name="Subtask" dataDxfId="3"/>
+    <tableColumn id="3" name="Kommentar" dataDxfId="2"/>
+    <tableColumn id="4" name="Bearbeiter" dataDxfId="1"/>
+    <tableColumn id="5" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1694,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,7 +1710,7 @@
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>6</v>
@@ -1753,7 +1723,7 @@
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F8" s="18" t="s">
         <v>6</v>
@@ -1766,7 +1736,7 @@
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>6</v>
@@ -1792,7 +1762,7 @@
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>6</v>
@@ -2081,10 +2051,10 @@
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="29" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>128</v>
@@ -2246,7 +2216,7 @@
         <v>115</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E46" s="17" t="s">
         <v>124</v>
@@ -2365,7 +2335,7 @@
         <v>128</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -2633,7 +2603,7 @@
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>6</v>
@@ -2646,7 +2616,7 @@
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>6</v>
@@ -2683,7 +2653,7 @@
         <v>20</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>6</v>
@@ -2696,7 +2666,7 @@
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>6</v>
@@ -2709,7 +2679,7 @@
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="24" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>6</v>
@@ -2722,7 +2692,7 @@
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>6</v>
@@ -2735,7 +2705,7 @@
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="24" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>6</v>
@@ -2748,7 +2718,7 @@
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>6</v>
@@ -2761,7 +2731,7 @@
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="24" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>6</v>
@@ -2774,7 +2744,7 @@
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>6</v>
@@ -2787,7 +2757,7 @@
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="24" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>6</v>
@@ -2800,7 +2770,7 @@
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>6</v>
@@ -2813,7 +2783,7 @@
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="24" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>6</v>
@@ -2826,7 +2796,7 @@
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F91" s="6" t="s">
         <v>6</v>
@@ -2839,7 +2809,7 @@
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="24" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>6</v>
@@ -3087,7 +3057,7 @@
       </c>
       <c r="D112" s="8"/>
       <c r="E112" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F112" s="25" t="s">
         <v>13</v>
@@ -3100,7 +3070,7 @@
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F113" s="6" t="s">
         <v>6</v>
@@ -3121,178 +3091,178 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F115:F1048576 F108:F111 F33 F37:F50 F52:F82 F1:F24 F96:F100">
-    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="49" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="50" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="51" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:F26">
-    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="46" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="47" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="48" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27:F30">
-    <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="43" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="44" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="45" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31:F32">
-    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="40" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="41" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="42" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F83:F84">
-    <cfRule type="cellIs" dxfId="38" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="34" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="35" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="36" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F85:F86">
-    <cfRule type="cellIs" dxfId="35" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="31" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="32" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="33" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87:F88">
-    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="28" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="29" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="30" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F89:F90">
-    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="25" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="26" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="27" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F91:F94">
-    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="23" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="24" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F112:F113">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F58:F62">
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F114">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:F36">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F102:F106">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated Tasklist with latest Issues
</commit_message>
<xml_diff>
--- a/Doku/Tasks.xlsx
+++ b/Doku/Tasks.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84944088-350F-4877-82C5-16A8A5910BB8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16140"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="148">
   <si>
     <t>Task</t>
   </si>
@@ -63,9 +62,6 @@
     <t>Login Page erstellen</t>
   </si>
   <si>
-    <t>Wartend</t>
-  </si>
-  <si>
     <t>Mit Sessionmanagement verknüpfen</t>
   </si>
   <si>
@@ -454,12 +450,27 @@
   </si>
   <si>
     <t>Benutzerhandbuch für BWLer</t>
+  </si>
+  <si>
+    <t>Icon Palette erweitern</t>
+  </si>
+  <si>
+    <t>Overlay Texte und Hover Effekte hinzufügen</t>
+  </si>
+  <si>
+    <t>Benachrichtigungsservice</t>
+  </si>
+  <si>
+    <t>Darstellung von Permissions über Icons</t>
+  </si>
+  <si>
+    <t>Eingeloggter Username mit Bild und Menü in Statusleiste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -756,7 +767,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1240,41 +1251,6 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1384,10 +1360,44 @@
       </border>
     </dxf>
     <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1404,14 +1414,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="B2:F112" totalsRowShown="0" headerRowDxfId="48" dataDxfId="49" headerRowBorderDxfId="57" tableBorderDxfId="56" totalsRowBorderDxfId="55">
-  <autoFilter ref="B2:F112" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B2:F117" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54" totalsRowBorderDxfId="53">
+  <autoFilter ref="B2:F117"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Subtask" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Kommentar" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Bearbeiter" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Status" dataDxfId="50"/>
+    <tableColumn id="1" name="Task" dataDxfId="52"/>
+    <tableColumn id="2" name="Subtask" dataDxfId="51"/>
+    <tableColumn id="3" name="Kommentar" dataDxfId="50"/>
+    <tableColumn id="4" name="Bearbeiter" dataDxfId="49"/>
+    <tableColumn id="5" name="Status" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1703,23 +1713,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F112"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F111" sqref="F111"/>
+    <sheetView tabSelected="1" topLeftCell="B100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="86.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="86.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="30" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" s="30" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
@@ -1727,7 +1737,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>2</v>
@@ -1736,7 +1746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
@@ -1745,72 +1755,72 @@
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="15"/>
       <c r="C6" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="15"/>
       <c r="C7" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="15"/>
       <c r="C8" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
@@ -1819,970 +1829,970 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="15"/>
       <c r="C10" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="15"/>
       <c r="C11" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="C12" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
       <c r="C13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>16</v>
-      </c>
       <c r="E13" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="17"/>
       <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="E15" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="15"/>
       <c r="C16" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15"/>
       <c r="C17" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="15"/>
       <c r="C18" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F18" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
       <c r="C23" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="15"/>
       <c r="C24" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
       <c r="C25" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F25" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="15"/>
       <c r="C26" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>43</v>
-      </c>
       <c r="E26" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="15"/>
       <c r="C27" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="15"/>
       <c r="C28" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="15"/>
       <c r="C29" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="15"/>
       <c r="C30" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="15"/>
       <c r="C31" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="15"/>
       <c r="C32" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="15"/>
       <c r="C33" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="15"/>
       <c r="C34" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F34" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="15"/>
       <c r="C35" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="15"/>
       <c r="C36" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="15"/>
       <c r="C37" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="15"/>
       <c r="C38" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F38" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="15"/>
       <c r="C39" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F39" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="15"/>
       <c r="C40" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="15"/>
       <c r="C41" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="15"/>
       <c r="C42" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="D42" s="20" t="s">
-        <v>113</v>
-      </c>
       <c r="E42" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="15"/>
       <c r="C43" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F43" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="15"/>
       <c r="C44" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="15"/>
       <c r="C45" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="15"/>
       <c r="C46" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F46" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="15"/>
       <c r="C47" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F47" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="15"/>
       <c r="C48" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F48" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="15"/>
       <c r="C49" s="20" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="D49" s="20"/>
-      <c r="E49" s="13" t="s">
-        <v>129</v>
+      <c r="E49" s="21" t="s">
+        <v>122</v>
       </c>
       <c r="F49" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="7" t="s">
+    <row r="50" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="15"/>
+      <c r="C50" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D50" s="20"/>
+      <c r="E50" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="15"/>
+      <c r="C51" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" s="20"/>
+      <c r="E51" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="17"/>
+      <c r="C53" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-    </row>
-    <row r="51" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="17"/>
-      <c r="C51" s="20" t="s">
+      <c r="D53" s="4"/>
+      <c r="E53" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="17"/>
+      <c r="C54" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="17"/>
-      <c r="C52" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F52" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="15"/>
-      <c r="C53" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D53" s="20"/>
-      <c r="E53" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F53" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="15"/>
-      <c r="C54" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D54" s="20"/>
+      <c r="D54" s="4"/>
       <c r="E54" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F54" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="15"/>
       <c r="C55" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D55" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="D55" s="20"/>
       <c r="E55" s="21" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F55" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="15"/>
       <c r="C56" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D56" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="D56" s="20"/>
       <c r="E56" s="21" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F56" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="15"/>
       <c r="C57" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D57" s="20"/>
+        <v>76</v>
+      </c>
+      <c r="D57" s="4"/>
       <c r="E57" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F57" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="15"/>
       <c r="C58" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D58" s="20"/>
+        <v>77</v>
+      </c>
+      <c r="D58" s="4"/>
       <c r="E58" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F58" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="15"/>
       <c r="C59" s="20" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="D59" s="20"/>
       <c r="E59" s="21" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F59" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="15"/>
-      <c r="C60" s="20" t="s">
-        <v>100</v>
+      <c r="C60" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="D60" s="20"/>
       <c r="E60" s="21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F60" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
-    </row>
-    <row r="62" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="15"/>
+      <c r="C61" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D61" s="20"/>
+      <c r="E61" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="15"/>
       <c r="C62" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E62" s="13" t="s">
-        <v>123</v>
+        <v>99</v>
+      </c>
+      <c r="D62" s="20"/>
+      <c r="E62" s="21" t="s">
+        <v>129</v>
       </c>
       <c r="F62" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="15"/>
-      <c r="C63" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D63" s="20"/>
-      <c r="E63" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="15"/>
       <c r="C64" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20" t="s">
-        <v>123</v>
+      <c r="E64" s="13" t="s">
+        <v>122</v>
       </c>
       <c r="F64" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="15"/>
       <c r="C65" s="20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D65" s="20"/>
-      <c r="E65" s="20" t="s">
-        <v>123</v>
+      <c r="E65" s="13" t="s">
+        <v>122</v>
       </c>
       <c r="F65" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="15"/>
       <c r="C66" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="D66" s="20" t="s">
-        <v>89</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D66" s="20"/>
       <c r="E66" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F66" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="17"/>
+    <row r="67" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="15"/>
       <c r="C67" s="20" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D67" s="20"/>
       <c r="E67" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F67" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="15"/>
       <c r="C68" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D68" s="20"/>
+        <v>86</v>
+      </c>
+      <c r="D68" s="20" t="s">
+        <v>88</v>
+      </c>
       <c r="E68" s="20" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F68" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="15"/>
+    <row r="69" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="17"/>
       <c r="C69" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D69" s="20"/>
       <c r="E69" s="20" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F69" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-    </row>
-    <row r="71" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="15"/>
+      <c r="C70" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="15"/>
       <c r="C71" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D71" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E71" s="21" t="s">
-        <v>123</v>
+        <v>90</v>
+      </c>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20" t="s">
+        <v>126</v>
       </c>
       <c r="F71" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="15"/>
-      <c r="C72" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D72" s="20"/>
-      <c r="E72" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="F72" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="15"/>
       <c r="C73" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D73" s="20"/>
-      <c r="E73" s="13" t="s">
-        <v>136</v>
+        <v>49</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E73" s="21" t="s">
+        <v>122</v>
       </c>
       <c r="F73" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="15"/>
       <c r="C74" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D74" s="20"/>
       <c r="E74" s="21" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="F74" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="10"/>
-    </row>
-    <row r="76" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="15"/>
+      <c r="C75" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D75" s="20"/>
+      <c r="E75" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="15"/>
       <c r="C76" s="20" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D76" s="20"/>
       <c r="E76" s="21" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="F76" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="15"/>
-      <c r="C77" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D77" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E77" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="F77" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="10"/>
+    </row>
+    <row r="78" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="15"/>
       <c r="C78" s="20" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="D78" s="20"/>
       <c r="E78" s="21" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="F78" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="15"/>
       <c r="C79" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D79" s="20"/>
-      <c r="E79" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D79" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E79" s="21" t="s">
         <v>137</v>
       </c>
       <c r="F79" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="15"/>
       <c r="C80" s="20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D80" s="20"/>
       <c r="E80" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F80" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="15"/>
       <c r="C81" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D81" s="20"/>
       <c r="E81" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F81" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="15"/>
       <c r="C82" s="20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D82" s="20"/>
       <c r="E82" s="21" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F82" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="15"/>
       <c r="C83" s="20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D83" s="20"/>
       <c r="E83" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F83" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="15"/>
       <c r="C84" s="20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D84" s="20"/>
       <c r="E84" s="21" t="s">
@@ -2792,360 +2802,425 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="15"/>
       <c r="C85" s="20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D85" s="20"/>
       <c r="E85" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F85" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="15"/>
       <c r="C86" s="20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D86" s="20"/>
       <c r="E86" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F86" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="15"/>
       <c r="C87" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D87" s="20"/>
       <c r="E87" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F87" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="15"/>
       <c r="C88" s="20" t="s">
         <v>64</v>
       </c>
       <c r="D88" s="20"/>
       <c r="E88" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F88" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="15"/>
       <c r="C89" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D89" s="20"/>
       <c r="E89" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F89" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="15"/>
       <c r="C90" s="20" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="D90" s="20"/>
-      <c r="E90" s="23" t="s">
-        <v>127</v>
+      <c r="E90" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="F90" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="17"/>
-      <c r="C91" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D91" s="4"/>
-      <c r="E91" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F91" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C92" s="7"/>
-      <c r="D92" s="7"/>
-      <c r="E92" s="7"/>
-      <c r="F92" s="7"/>
-    </row>
-    <row r="93" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="15"/>
+      <c r="C91" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D91" s="20"/>
+      <c r="E91" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="F91" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="15"/>
+      <c r="C92" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D92" s="20"/>
+      <c r="E92" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F92" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="17"/>
       <c r="C93" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D93" s="4"/>
-      <c r="E93" s="18" t="s">
-        <v>123</v>
+      <c r="E93" s="24" t="s">
+        <v>126</v>
       </c>
       <c r="F93" s="25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B94" s="17"/>
-      <c r="C94" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D94" s="4"/>
-      <c r="E94" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="F94" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+    </row>
+    <row r="95" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="17"/>
       <c r="C95" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F95" s="25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="15"/>
-      <c r="C96" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="D96" s="20"/>
-      <c r="E96" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="F96" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B97" s="15"/>
-      <c r="C97" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="D97" s="20"/>
-      <c r="E97" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="F97" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B98" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C98" s="8"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="9"/>
-      <c r="F98" s="10"/>
-    </row>
-    <row r="99" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="17"/>
+      <c r="C96" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D96" s="4"/>
+      <c r="E96" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="F96" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="17"/>
+      <c r="C97" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D97" s="4"/>
+      <c r="E97" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="F97" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="15"/>
+      <c r="C98" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D98" s="20"/>
+      <c r="E98" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F98" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="15"/>
       <c r="C99" s="20" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D99" s="20"/>
       <c r="E99" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F99" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B100" s="15"/>
-      <c r="C100" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="D100" s="20"/>
-      <c r="E100" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="F100" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="10"/>
+    </row>
+    <row r="101" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="15"/>
       <c r="C101" s="20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D101" s="20"/>
       <c r="E101" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F101" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="15"/>
       <c r="C102" s="20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D102" s="20"/>
       <c r="E102" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F102" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="15"/>
       <c r="C103" s="20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D103" s="20"/>
       <c r="E103" s="21" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F103" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B104" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C104" s="8"/>
-      <c r="D104" s="8"/>
-      <c r="E104" s="9"/>
-      <c r="F104" s="10"/>
-    </row>
-    <row r="105" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="15"/>
+      <c r="C104" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D104" s="20"/>
+      <c r="E104" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F104" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="15"/>
       <c r="C105" s="20" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="D105" s="20"/>
       <c r="E105" s="21" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F105" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="15"/>
-      <c r="C106" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D106" s="20"/>
-      <c r="E106" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="F106" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="107" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="10"/>
+    </row>
+    <row r="107" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="15"/>
       <c r="C107" s="20" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="D107" s="20"/>
       <c r="E107" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F107" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="15"/>
       <c r="C108" s="20" t="s">
         <v>104</v>
       </c>
       <c r="D108" s="20"/>
       <c r="E108" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F108" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B109" s="17"/>
-      <c r="C109" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D109" s="4"/>
-      <c r="E109" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="F109" s="25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="110" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="15"/>
+      <c r="C109" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D109" s="20"/>
+      <c r="E109" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F109" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="15"/>
       <c r="C110" s="20" t="s">
-        <v>143</v>
+        <v>103</v>
       </c>
       <c r="D110" s="20"/>
       <c r="E110" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="F110" s="25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="111" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+      <c r="F110" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="15"/>
       <c r="C111" s="20" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="D111" s="20"/>
       <c r="E111" s="21" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="F111" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="2:6" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B112" s="3"/>
-      <c r="C112" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4" t="s">
-        <v>126</v>
+    <row r="112" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="15"/>
+      <c r="C112" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="D112" s="20"/>
+      <c r="E112" s="21" t="s">
+        <v>122</v>
       </c>
       <c r="F112" s="19" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="113" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="17"/>
+      <c r="C113" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D113" s="4"/>
+      <c r="E113" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="F113" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="15"/>
+      <c r="C114" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D114" s="20"/>
+      <c r="E114" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F114" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="15"/>
+      <c r="C115" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D115" s="20"/>
+      <c r="E115" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F115" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="15"/>
+      <c r="C116" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D116" s="20"/>
+      <c r="E116" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F116" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" s="6" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="3"/>
+      <c r="C117" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F117" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F113:F1048576 F105:F108 F30 F34:F47 F49:F79 F93:F97 F1:F21">
+  <conditionalFormatting sqref="F118:F1048576 F107:F112 F30 F34:F47 F51:F81 F95:F99 F1:F21">
     <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
@@ -3189,7 +3264,7 @@
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F80:F81">
+  <conditionalFormatting sqref="F82:F83">
     <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
@@ -3200,7 +3275,7 @@
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F82:F83">
+  <conditionalFormatting sqref="F84:F85">
     <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
@@ -3211,7 +3286,7 @@
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F84:F85">
+  <conditionalFormatting sqref="F86:F87">
     <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
@@ -3222,7 +3297,7 @@
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F86:F87">
+  <conditionalFormatting sqref="F88:F89">
     <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
@@ -3233,7 +3308,7 @@
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F88:F91">
+  <conditionalFormatting sqref="F90:F93">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
@@ -3244,7 +3319,7 @@
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F109:F111">
+  <conditionalFormatting sqref="F113:F116">
     <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
@@ -3255,7 +3330,7 @@
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F55:F59">
+  <conditionalFormatting sqref="F57:F61">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
@@ -3266,7 +3341,7 @@
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F112">
+  <conditionalFormatting sqref="F117">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
@@ -3288,7 +3363,7 @@
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F48">
+  <conditionalFormatting sqref="F48:F50">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
@@ -3299,7 +3374,7 @@
       <formula>"Offen"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F99:F103">
+  <conditionalFormatting sqref="F101:F105">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Wartend"</formula>
     </cfRule>
@@ -3322,7 +3397,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D77" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D79" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -3333,24 +3408,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>